<commit_message>
Final version, demo rec delivered to Jules
</commit_message>
<xml_diff>
--- a/input/Fingerprint experiments.xlsx
+++ b/input/Fingerprint experiments.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlbkm/fingerprint_matching/input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A51AF05-4EF9-0947-A857-B8835DE188E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Program</t>
   </si>
@@ -22,99 +31,7 @@
     <t>Gender Equality and Inclusion</t>
   </si>
   <si>
-    <t>Gender Equality and Social Inclusion
-Accelerator
-Full design document
-September 2024
-2
-Table of Contents
-Table of Contents................................................................................................................... 2
-List of acronyms..................................................................................................................... 3
-1. Executive Summary............................................................................................................ 4
-2. High-level vision in response to challenges and megatrends ................................................ 5
-2.1. Challenges and megatrends ......................................................................................... 5
-2.2. High-level vision........................................................................................................... 5
-2.3. What is new in this Accelerator? ................................................................................... 6
-3. Use-Case-based prioritization ............................................................................................ 6
-4. Comparative advantage...................................................................................................... 9
-5. Program-/Accelerator-level theory of change (TOC)............................................................ 12
-6. Areas of Work................................................................................................................... 15
-6.1. Introduction to Areas of Work ..................................................................................... 15
-6.2. Area of Work 1: Accelerating Solutions for impact ....................................................... 18
-6.3. Area of Work 2: Accelerating CHANGE ........................................................................ 34
-7. Boundaries and linkages with other components of the Portfolio........................................ 39
-8. Monitoring, Evaluation, Learning, and Impact Assessment (MELIA) .................................... 42
-8.1. Monitoring, Evaluation, and Learning (MEL)................................................................. 42
-8.2. Impact Assessment (IA).............................................................................................. 43
-9. Capacity sharing .............................................................................................................. 44
-9.1. Training and development of resources....................................................................... 44
-9.2. Knowledge sharing for social learning ......................................................................... 46
-10. Gender and social inclusion............................................................................................ 46
-11. Climate change .............................................................................................................. 46
-12. Risk management........................................................................................................... 48
-13. Funding sources............................................................................................................. 48
-Annex - Pooled funding......................................................................................................... 54
-References .......................................................................................................................... 57
-3
-List of acronyms
-ADB Asian Development Bank
-AfDB African Development Bank
-AFS Agrifood systems
-AGRA Alliance for a Green Revolution in Africa
-AoW Area of Work
-APAARI Asia-Pacific Association of Agricultural Research Institutions
-AR4D Agricultural research for development
-AWARD African Women in Agricultural Research and Development
-CA Comparative advantage
-CARE Cooperative for Assistance and Relief Everywhere
-CG CGIAR
-CNA Capacity and needs assessment
-CSA Climate-smart agriculture
-CSO Civil society organization
-FAO Food and Agriculture Organization of the United Nations
-FARA Forum for Agricultural Research in Africa
-FHI 360 Family Health International
-FLW Food, land and water
-FLWS Food, land and water systems
-GESI Gender equality and social inclusion
-GREAT Gender-Responsive Researchers Equipped for Agricultural
-Transformation
-GT Gender-transformative
-GTA Gender-transformative approach
-GYSI Gender, Youth and Social Inclusion
-HER+ Gender Equality Initiative
-HLO High-level output
-IA Impact assessment
-ICAR Indian Council of Agricultural Research
-IFAD International Fund for Agricultural Development
-IP&amp;LC Indigenous peoples and local communities
-KALRO Kenya Agricultural and Livestock Research Organization
-MEL Monitoring, evaluation and learning
-MELIA Monitoring, evaluation, learning, and impact assessment
-NARES National agricultural research and extension systems
-NARS National agricultural research systems
-R4D Research for development
-SAPLING Sustainable Animal Productivity for Livelihoods, Nutrition, and Gender
-Inclusion
-SDG Sustainable development goal
-SEARCA Southeast Asian Regional Center for Graduate Study and Research in
-Agriculture
-SI MFS Sustainable Intensification of Mixed Farming Systems
-Science
-Program
-Science Program
-STIBs Sociotechnical innovation bundles
-TOC Theory of change
-TVET Technical and vocational education and training
-UN United Nations
-VSS Voluntary sustainability standards
-WEAI Women’s Empowerment in Agriculture Index
-WFP
-YPARD
-World Food Program
-Young Professionals for Agricultural Development
-4
-1. Executive Summary
+    <t xml:space="preserve">1. Executive Summary
 To address the pressing global challenges and megatrends in gender and social equality within
 food, land and water systems (FLWS) under a changing climate, CGIAR recognizes the need
 to invest in a Gender Equality and Social Inclusion Accelerator. This Accelerator has a dual
@@ -455,106 +372,81 @@
 A core principle of the Accelerator is the co-design of solutions and their implementation in a
 participatory manner. Building on experiences from the past portfolio, AoW2 expands work on
 targeting, demand signaling, and evidence synthesis and facilitation of uptake. The joint
-identification of innovations will lead to solutions and form a basis for developing metrics to
-assess impact, and for building capacity to take up solutions and create positive feedback
-loops for learning and adjustment.
-The two AoWs address these overarching research questions:
-• What are the most effective and scalable solutions for advancing gender equality and
-engaging youth to deliver on inclusive and just FLWS?
-• What evidence, strategies and policies can enable structural change to drive
-integration of GESI in AR4D organizations and catalyze equality in FLWS?
-14
-The Accelerator’s major outputs include:
-• Co-developed and tested solutions to advance GESI and youth engagement to
-catalyze inclusive FLWS.
-• Solutions to support women’s empowerment and resilience in FLWS under a changing
-climate.
-• Increased understanding of youth’s role in FLWS by CGIAR and partners.
-• Advanced methods for intersectional analysis that enable effective targeting and
-scaling of FLWS solutions.
-• Metrics and toolkits to capture GESI and youth outcomes and impacts in FLWS.
-• Large datasets and analytics, and decision-support systems to enable evidence-based
-strategic planning and policymaking for equitable and resilient FLWS.
-• Enhanced capacities to use and scale GESI approaches, methods and solutions for
-FLWS transformation.
-• Institutional structures and incentives that facilitate GESI inclusion in AR4D.
-The Accelerator aligns the priorities of both AoWs with national, regional and global demands.
-Partnerships are key to accelerating change and reaching the Accelerator’s 2030 and
-intermediary outcomes. Within CGIAR, working with the Science Programs (Science
-Programs), the Scaling Program and the Accelerators will require an iterative relationship
-where the Science Programs contribute to the thematic AoWs of the Gender and Social
-Inclusion Accelerator; while the Accelerator contributes methodologies, evidence, tools,
-approaches, best practices, and more, to raise the ambition of the Science Programs on GESI
-and drive a coherent CGIAR-wide GESI research agenda.
-Beyond CGIAR, the Accelerator harnesses high-level support, fosters strategic partnerships,
-and influences global discourse to build an enabling external environment for GESI in FLWS
-research through effective communication and engagement. It builds and sustains global
-coalitions and networks to accelerate the impact of GESI initiatives on a broader scale.
-The Accelerator works closely with bilateral projects, United States Agency for International
-Development Innovation Labs, German Agency for International Cooperation (GIZ) and
-International Fund for Agricultural Development (IFAD) programs, among others, to advance
-positive GESI outcomes in FLWS. Relevant research and outcomes is also driven by strong
-engagement with research networks like FARA and its sub-regional organizations, Asia-Pacific
-Association of Agricultural Research Institutions (APAARI), Southeast Asian Regional Center
-for Graduate Study and Research in Agriculture (SEARCA) and National agricultural research
-systems (NARS) like Indian Council of Agricultural Research (ICAR), Brazilian Agricultural
-Research Corporation, Chinese Academy of Agricultural Sciences, Uganda National
-Agricultural Research Organization, Kenya Agricultural and Livestock Research Organization
-(KALRO), and Ethiopian Institute of Agricultural Research.
-Moreover, the Accelerator engages with national governments and multilateral organizations
-to understand their information needs in support of evidence-based policymaking and program
-design, and their preferences for accessing this evidence. The Accelerator’s work with global
-partners — such as World Bank, Food and Agriculture Organization of the United Nations
-(FAO), IFAD, Asian Development Bank (ADB), African Development Bank (AfDB), and Alliance
-for a Green Revolution in Africa (AGRA) — builds on previous successful engagement, such
-as collaborations on the Status of Women in Agrifood Systems and the Voluntary Guidelines
-on Gender Equality and Women’s and Girls’ Empowerment in the Context of Food Security
-and Nutrition. With its presence across multiple Centers and connections to a broad spectrum
-of actors, the Accelerator is poised to continue to influence agricultural innovation to become
-more inclusive.
-15
-Through engagement with these partners, the Accelerator:
-• Develops new methods and metrics to advance and measure changes in gender
-equality, and the inclusion of IP&amp;LC, youth and socially excluded groups.
-• Develops analytics and decision support systems to inform policy and program design
-and gain the ability use evidence and data.
-• Collaborates with capacity development organizations to build human and social
-capital in CGIAR and partner organizations to enable them to use the new approaches
-and metrics developed.
-• Nurtures communities of practice around GESI and youth, incorporating agricultural
-universities and research networks globally (e.g., Cornell University, Royal Roads
-University, Makerere University, GREAT, AWARD, AIT, SEARCA, FARA, APAARI).
-• Identifies what works, where, for whom, and under what conditions as well as costeffective GESI solutions for FLWS — in partnership with research organizations with
-a strong background on impact assessments, such as J-PAL, the Africa Gender
-Innovation Lab, and Airbel Impact Lab.
-• Synthesizes evidence and communicates it to target audiences, including through
-Evidence Explainers, infographics, and other innovative and strategic communication
-products, to inspire and enable other organizations to scale these solutions for
-equitable FLWS.
-• Engages with global policy processes such as UNFCCC, CBD and United Nations
-Convention to Combat Desertification to provide evidence-based recommendations
-and strategies.
-• Monitors and manages evidence uptake to facilitate scaling.
-• Supports change in CGIAR institutional frameworks to systematically address gender
-equality and social inclusion when setting research priorities, defining partnerships and
-making decisions with partners to ensure intentionality on GESI in technology design,
-delivery and scaling.</t>
+identification of innovations will lead to solutions </t>
+  </si>
+  <si>
+    <t>Executive Summary
+Digital transformation offers solutions to the complex challenges facing food, land and water
+(FLW) systems through real-time monitoring, advanced data analytics, and connecting
+stakeholders at scale. CGIAR has a key role to play in localization digital frontier technologies
+by adapting these solutions to the Global South while promoting digital inclusivity and equitable
+access to technology. To do so, CGIAR must adapt at an institutional and cultural level,
+developing new partnerships and workflows to adopt digital advances.
+The Digital Transformation Accelerator will work with CGIAR and partners to co-design inclusive
+solutions building on advances in modeling, artificial intelligence (AI), machine learning, and big
+data analytics. Outcomes such as improved decision-making, enabling policies and
+investments, and increased adoption of digital solutions by stakeholders and actors will provide
+a foundation to address CGIAR’s five Impact Areas more effectively.
+Digital Transformation will continue select research and innovation from CGIAR Initiatives on
+Digital Innovation, Breeding Resources, and Excellence in Agronomy, CGIAR Digital &amp; Data
+Group, and bilaterally supported digital research and development projects across Centers,
+based on use case-based prioritization. Addressing data challenges identified in the previous
+Portfolio, Data Ecosystem (AoW1) will enhance data sharing across Centers and develop
+advanced analytics in a collaborative way, focusing on the implementation of FAIR (Findable,
+Accessible, Interoperable, and Reusable) principles, inclusive governance, and cultural change
+processes. Through Action Lab (AoW2), Digital Transformation continues innovations from the
+Digital Innovation Initiative, co-developing prioritized use cases with stakeholders, accelerating
+the development of digital and AI-driven innovations and insights, and addressing inclusivity
+through citizen science, gender and social inclusion, and human-centered design approaches.
+This process will largely define the targeted geographic area. Digital Futures (AoW3) will
+develop a series of foresight case studies to identify digital frontier technologies with the
+opportunity to transform FLW systems, facilitating critical discussions to address the risks of
+widening technological divides and inequalities. Enabling Environment (AoW4) will establish a
+decentralized network of Digital Innovation Hubs for CGIAR and its stakeholders to access
+expertise, resources, and collaboration opportunities. It will lead where digital transformation
+intersects with gender and social inclusion, scaling and capacity sharing, ethics, data
+governance, behavioral change, and business development. Digital Transformation will also
+provision a digital core of infrastructure, tools, and communities of practice, as the backbone of
+the digital transformation of CGIAR.
+Driven by strong demand identified in Listening Sessions in 14 countries in the Global South,
+emerging use cases include AI models, especially large language models, to interact with
+CGIAR’s data and knowledge products, including agronomic and crop breeding data for resilient
+productivity, bringing in citizen science and engaging youth, and embedding a data-to-analytics
+workflow across all Programs. Use cases matured in the Accelerator will scale through the
+Scaling for Impact Program for broader implementation.
+Success for the Accelerator requires institutional support and significant resources including
+technical talent, domain knowledge, infrastructure, partnerships, datasets, and capacity building.
+While CGIAR holds comparative advantages in these areas, other partners will be brought in to
+leverage specific advantages in the digital domain on a mutual benefit basis, whether it be
+greater financial resources and technological expertise, or greater understanding of local</t>
+  </si>
+  <si>
+    <t>Digital Transformation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -563,36 +455,50 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -782,20 +688,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="107.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,15 +717,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>